<commit_message>
full function version change source to google. Google only have Close index.
</commit_message>
<xml_diff>
--- a/files/Stocks_Simple.xlsx
+++ b/files/Stocks_Simple.xlsx
@@ -14,18 +14,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>INTC</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>AMZN</t>
   </si>
   <si>
+    <t>r_AMZN</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>r_GOOG</t>
+  </si>
+  <si>
     <t>MSFT</t>
   </si>
   <si>
-    <t>GOOG</t>
+    <t>r_MSFT</t>
+  </si>
+  <si>
+    <t>CTRP</t>
+  </si>
+  <si>
+    <t>r_CTRP</t>
+  </si>
+  <si>
+    <t>VMW</t>
+  </si>
+  <si>
+    <t>r_VMW</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>r_JD</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>r_BABA</t>
   </si>
   <si>
     <t>Date</t>
@@ -392,15 +422,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -414,158 +444,813 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="2">
+        <v>42373</v>
+      </c>
+      <c r="B2">
+        <v>636.99</v>
+      </c>
+      <c r="D2">
+        <v>741.84</v>
+      </c>
+      <c r="F2">
+        <v>54.8</v>
+      </c>
+      <c r="H2">
+        <v>45.23</v>
+      </c>
+      <c r="J2">
+        <v>56.3</v>
+      </c>
+      <c r="L2">
+        <v>29.53</v>
+      </c>
+      <c r="N2">
+        <v>76.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="2">
+        <v>42403</v>
+      </c>
+      <c r="B3">
+        <v>531.0700000000001</v>
+      </c>
+      <c r="C3">
+        <v>-0.1662820452440383</v>
+      </c>
+      <c r="D3">
+        <v>726.95</v>
+      </c>
+      <c r="E3">
+        <v>-0.02007171357705162</v>
+      </c>
+      <c r="F3">
+        <v>52.16</v>
+      </c>
+      <c r="G3">
+        <v>-0.04817518248175179</v>
+      </c>
+      <c r="H3">
+        <v>39.9</v>
+      </c>
+      <c r="I3">
+        <v>-0.1178421401724519</v>
+      </c>
+      <c r="J3">
+        <v>44.96</v>
+      </c>
+      <c r="K3">
+        <v>-0.2014209591474244</v>
+      </c>
+      <c r="L3">
+        <v>23.81</v>
+      </c>
+      <c r="M3">
+        <v>-0.193701320690823</v>
+      </c>
+      <c r="N3">
+        <v>63.44</v>
+      </c>
+      <c r="O3">
+        <v>-0.1727735037162603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="2">
+        <v>42433</v>
+      </c>
+      <c r="B4">
+        <v>575.14</v>
+      </c>
+      <c r="C4">
+        <v>0.08298341084979377</v>
+      </c>
+      <c r="D4">
+        <v>710.89</v>
+      </c>
+      <c r="E4">
+        <v>-0.02209230345966029</v>
+      </c>
+      <c r="F4">
+        <v>52.03</v>
+      </c>
+      <c r="G4">
+        <v>-0.002492331288343475</v>
+      </c>
+      <c r="H4">
+        <v>40.02</v>
+      </c>
+      <c r="I4">
+        <v>0.003007518796992681</v>
+      </c>
+      <c r="J4">
+        <v>49.45</v>
+      </c>
+      <c r="K4">
+        <v>0.09986654804270456</v>
+      </c>
+      <c r="L4">
+        <v>26.48</v>
+      </c>
+      <c r="M4">
+        <v>0.1121377572448552</v>
+      </c>
+      <c r="N4">
+        <v>72.22</v>
+      </c>
+      <c r="O4">
+        <v>0.1383984867591426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="2">
+        <v>42465</v>
+      </c>
+      <c r="B5">
+        <v>586.14</v>
+      </c>
+      <c r="C5">
+        <v>0.01912577807142601</v>
+      </c>
+      <c r="D5">
+        <v>737.8</v>
+      </c>
+      <c r="E5">
+        <v>0.03785395771497702</v>
+      </c>
+      <c r="F5">
+        <v>54.56</v>
+      </c>
+      <c r="G5">
+        <v>0.04862579281183943</v>
+      </c>
+      <c r="H5">
+        <v>43.71</v>
+      </c>
+      <c r="I5">
+        <v>0.09220389805097451</v>
+      </c>
+      <c r="J5">
+        <v>50.7</v>
+      </c>
+      <c r="K5">
+        <v>0.02527805864509602</v>
+      </c>
+      <c r="L5">
+        <v>26.52</v>
+      </c>
+      <c r="M5">
+        <v>0.001510574018126931</v>
+      </c>
+      <c r="N5">
+        <v>77.31999999999999</v>
+      </c>
+      <c r="O5">
+        <v>0.07061755746330656</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="2">
+        <v>42494</v>
+      </c>
+      <c r="B6">
+        <v>670.9</v>
+      </c>
+      <c r="C6">
+        <v>0.1446070904562049</v>
+      </c>
+      <c r="D6">
+        <v>695.7</v>
+      </c>
+      <c r="E6">
+        <v>-0.0570615342911357</v>
+      </c>
+      <c r="F6">
+        <v>49.87</v>
+      </c>
+      <c r="G6">
+        <v>-0.08596041055718484</v>
+      </c>
+      <c r="H6">
+        <v>43.62</v>
+      </c>
+      <c r="I6">
+        <v>-0.002059025394646641</v>
+      </c>
+      <c r="J6">
+        <v>55.36</v>
+      </c>
+      <c r="K6">
+        <v>0.09191321499013805</v>
+      </c>
+      <c r="L6">
+        <v>24.22</v>
+      </c>
+      <c r="M6">
+        <v>-0.0867269984917044</v>
+      </c>
+      <c r="N6">
+        <v>75.81999999999999</v>
+      </c>
+      <c r="O6">
+        <v>-0.01939989653388519</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="2">
+        <v>42524</v>
+      </c>
+      <c r="B7">
+        <v>725.54</v>
+      </c>
+      <c r="C7">
+        <v>0.08144283797883434</v>
+      </c>
+      <c r="D7">
+        <v>722.34</v>
+      </c>
+      <c r="E7">
+        <v>0.03829236739974129</v>
+      </c>
+      <c r="F7">
+        <v>51.79</v>
+      </c>
+      <c r="G7">
+        <v>0.03850010026067774</v>
+      </c>
+      <c r="H7">
+        <v>43.84</v>
+      </c>
+      <c r="I7">
+        <v>0.005043558000917159</v>
+      </c>
+      <c r="J7">
+        <v>62.08</v>
+      </c>
+      <c r="K7">
+        <v>0.1213872832369942</v>
+      </c>
+      <c r="L7">
+        <v>22.98</v>
+      </c>
+      <c r="M7">
+        <v>-0.05119735755573895</v>
+      </c>
+      <c r="N7">
+        <v>76.62</v>
+      </c>
+      <c r="O7">
+        <v>0.01055130572408358</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="2">
+        <v>42556</v>
+      </c>
+      <c r="B8">
+        <v>728.1</v>
+      </c>
+      <c r="C8">
+        <v>0.003528406428315645</v>
+      </c>
+      <c r="D8">
+        <v>694.49</v>
+      </c>
+      <c r="E8">
+        <v>-0.03855525098983859</v>
+      </c>
+      <c r="F8">
+        <v>51.17</v>
+      </c>
+      <c r="G8">
+        <v>-0.01197142305464372</v>
+      </c>
+      <c r="H8">
+        <v>40.66</v>
+      </c>
+      <c r="I8">
+        <v>-0.07253649635036508</v>
+      </c>
+      <c r="J8">
+        <v>56.59</v>
+      </c>
+      <c r="K8">
+        <v>-0.08843427835051543</v>
+      </c>
+      <c r="L8">
+        <v>20.86</v>
+      </c>
+      <c r="M8">
+        <v>-0.09225413402959104</v>
+      </c>
+      <c r="N8">
+        <v>78.97</v>
+      </c>
+      <c r="O8">
+        <v>0.03067084312190027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="2">
+        <v>42585</v>
+      </c>
+      <c r="B9">
+        <v>754.64</v>
+      </c>
+      <c r="C9">
+        <v>0.03645103694547447</v>
+      </c>
+      <c r="D9">
+        <v>773.1799999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.1133061671154372</v>
+      </c>
+      <c r="F9">
+        <v>56.97</v>
+      </c>
+      <c r="G9">
+        <v>0.1133476646472542</v>
+      </c>
+      <c r="H9">
+        <v>42.5</v>
+      </c>
+      <c r="I9">
+        <v>0.04525332021642892</v>
+      </c>
+      <c r="J9">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.2440360487718678</v>
+      </c>
+      <c r="L9">
+        <v>21.73</v>
+      </c>
+      <c r="M9">
+        <v>0.04170661553211885</v>
+      </c>
+      <c r="N9">
+        <v>83.67</v>
+      </c>
+      <c r="O9">
+        <v>0.05951627200202614</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="2">
+        <v>42614</v>
+      </c>
+      <c r="B10">
+        <v>770.62</v>
+      </c>
+      <c r="C10">
+        <v>0.02117565991731163</v>
+      </c>
+      <c r="D10">
+        <v>768.78</v>
+      </c>
+      <c r="E10">
+        <v>-0.005690783517421583</v>
+      </c>
+      <c r="F10">
+        <v>57.59</v>
+      </c>
+      <c r="G10">
+        <v>0.01088292083552744</v>
+      </c>
+      <c r="H10">
+        <v>48.96</v>
+      </c>
+      <c r="I10">
+        <v>0.1519999999999999</v>
+      </c>
+      <c r="J10">
+        <v>73.78</v>
+      </c>
+      <c r="K10">
+        <v>0.04801136363636349</v>
+      </c>
+      <c r="L10">
+        <v>25.71</v>
+      </c>
+      <c r="M10">
+        <v>0.1831569259088817</v>
+      </c>
+      <c r="N10">
+        <v>97.42</v>
+      </c>
+      <c r="O10">
+        <v>0.1643360822277997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="2">
+        <v>42646</v>
+      </c>
+      <c r="B11">
+        <v>836.74</v>
+      </c>
+      <c r="C11">
+        <v>0.08580104331577165</v>
+      </c>
+      <c r="D11">
+        <v>772.5599999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.004916881292437392</v>
+      </c>
+      <c r="F11">
+        <v>57.42</v>
+      </c>
+      <c r="G11">
+        <v>-0.00295190137176593</v>
+      </c>
+      <c r="H11">
+        <v>46.95</v>
+      </c>
+      <c r="I11">
+        <v>-0.04105392156862742</v>
+      </c>
+      <c r="J11">
+        <v>73.61</v>
+      </c>
+      <c r="K11">
+        <v>-0.002304147465437834</v>
+      </c>
+      <c r="L11">
+        <v>26.11</v>
+      </c>
+      <c r="M11">
+        <v>0.0155581485803189</v>
+      </c>
+      <c r="N11">
+        <v>105.38</v>
+      </c>
+      <c r="O11">
+        <v>0.08170806815848897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="2">
+        <v>42675</v>
+      </c>
+      <c r="B12">
+        <v>785.41</v>
+      </c>
+      <c r="C12">
+        <v>-0.06134522073762461</v>
+      </c>
+      <c r="D12">
+        <v>783.61</v>
+      </c>
+      <c r="E12">
+        <v>0.01430309619964798</v>
+      </c>
+      <c r="F12">
+        <v>59.8</v>
+      </c>
+      <c r="G12">
+        <v>0.04144897248345525</v>
+      </c>
+      <c r="H12">
+        <v>43.41</v>
+      </c>
+      <c r="I12">
+        <v>-0.07539936102236433</v>
+      </c>
+      <c r="J12">
+        <v>77.97</v>
+      </c>
+      <c r="K12">
+        <v>0.05923108273332423</v>
+      </c>
+      <c r="L12">
+        <v>25.31</v>
+      </c>
+      <c r="M12">
+        <v>-0.0306396016851781</v>
+      </c>
+      <c r="N12">
+        <v>101.15</v>
+      </c>
+      <c r="O12">
+        <v>-0.0401404441070411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="2">
+        <v>42705</v>
+      </c>
+      <c r="B13">
+        <v>743.65</v>
+      </c>
+      <c r="C13">
+        <v>-0.053169682076877</v>
+      </c>
+      <c r="D13">
+        <v>747.92</v>
+      </c>
+      <c r="E13">
+        <v>-0.04554561580378003</v>
+      </c>
+      <c r="F13">
+        <v>59.2</v>
+      </c>
+      <c r="G13">
+        <v>-0.01003344481605339</v>
+      </c>
+      <c r="H13">
+        <v>44.83</v>
+      </c>
+      <c r="I13">
+        <v>0.03271135683022353</v>
+      </c>
+      <c r="J13">
+        <v>78.04000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.0008977811978967409</v>
+      </c>
+      <c r="L13">
+        <v>26.3</v>
+      </c>
+      <c r="M13">
+        <v>0.03911497431845135</v>
+      </c>
+      <c r="N13">
+        <v>89.86</v>
+      </c>
+      <c r="O13">
+        <v>-0.1116164112703906</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="2">
         <v>42738</v>
       </c>
-      <c r="B2">
-        <v>36.599998</v>
-      </c>
-      <c r="C2">
-        <v>753.669983</v>
-      </c>
-      <c r="D2">
-        <v>62.580002</v>
-      </c>
-      <c r="E2">
-        <v>786.1400150000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
-        <v>42739</v>
-      </c>
-      <c r="B3">
-        <v>36.41</v>
-      </c>
-      <c r="C3">
-        <v>757.179993</v>
-      </c>
-      <c r="D3">
-        <v>62.299999</v>
-      </c>
-      <c r="E3">
-        <v>786.900024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
-        <v>42740</v>
-      </c>
-      <c r="B4">
-        <v>36.349998</v>
-      </c>
-      <c r="C4">
-        <v>780.450012</v>
-      </c>
-      <c r="D4">
-        <v>62.299999</v>
-      </c>
-      <c r="E4">
-        <v>794.02002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2">
-        <v>42741</v>
-      </c>
-      <c r="B5">
-        <v>36.48</v>
-      </c>
-      <c r="C5">
-        <v>795.98999</v>
-      </c>
-      <c r="D5">
-        <v>62.84</v>
-      </c>
-      <c r="E5">
-        <v>806.150024</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2">
-        <v>42744</v>
-      </c>
-      <c r="B6">
-        <v>36.610001</v>
-      </c>
-      <c r="C6">
-        <v>796.919983</v>
-      </c>
-      <c r="D6">
-        <v>62.639999</v>
-      </c>
-      <c r="E6">
-        <v>806.650024</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2">
-        <v>42745</v>
-      </c>
-      <c r="B7">
-        <v>36.540001</v>
-      </c>
-      <c r="C7">
-        <v>795.900024</v>
-      </c>
-      <c r="D7">
-        <v>62.619999</v>
-      </c>
-      <c r="E7">
-        <v>804.789978</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2">
-        <v>42746</v>
-      </c>
-      <c r="B8">
-        <v>36.950001</v>
-      </c>
-      <c r="C8">
-        <v>799.02002</v>
-      </c>
-      <c r="D8">
-        <v>63.189999</v>
-      </c>
-      <c r="E8">
-        <v>807.909973</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2">
-        <v>42747</v>
-      </c>
-      <c r="B9">
-        <v>36.709999</v>
-      </c>
-      <c r="C9">
-        <v>813.6400150000001</v>
-      </c>
-      <c r="D9">
-        <v>62.610001</v>
-      </c>
-      <c r="E9">
-        <v>806.3599849999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2">
-        <v>42748</v>
-      </c>
-      <c r="B10">
-        <v>36.790001</v>
-      </c>
-      <c r="C10">
-        <v>817.1400150000001</v>
-      </c>
-      <c r="D10">
-        <v>62.700001</v>
-      </c>
-      <c r="E10">
-        <v>807.880005</v>
+      <c r="B14">
+        <v>753.67</v>
+      </c>
+      <c r="C14">
+        <v>0.01347408054864507</v>
+      </c>
+      <c r="D14">
+        <v>786.14</v>
+      </c>
+      <c r="E14">
+        <v>0.05110172210931663</v>
+      </c>
+      <c r="F14">
+        <v>62.58</v>
+      </c>
+      <c r="G14">
+        <v>0.05709459459459443</v>
+      </c>
+      <c r="H14">
+        <v>40.49</v>
+      </c>
+      <c r="I14">
+        <v>-0.09681017175998208</v>
+      </c>
+      <c r="J14">
+        <v>78.88</v>
+      </c>
+      <c r="K14">
+        <v>0.01076371091747808</v>
+      </c>
+      <c r="L14">
+        <v>25.82</v>
+      </c>
+      <c r="M14">
+        <v>-0.01825095057034221</v>
+      </c>
+      <c r="N14">
+        <v>88.59999999999999</v>
+      </c>
+      <c r="O14">
+        <v>-0.01402181170710004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="2">
+        <v>42768</v>
+      </c>
+      <c r="B15">
+        <v>839.95</v>
+      </c>
+      <c r="C15">
+        <v>0.1144798121193626</v>
+      </c>
+      <c r="D15">
+        <v>798.53</v>
+      </c>
+      <c r="E15">
+        <v>0.01576055155570244</v>
+      </c>
+      <c r="F15">
+        <v>63.17</v>
+      </c>
+      <c r="G15">
+        <v>0.009427932246724335</v>
+      </c>
+      <c r="H15">
+        <v>42.79</v>
+      </c>
+      <c r="I15">
+        <v>0.05680414917263521</v>
+      </c>
+      <c r="J15">
+        <v>88</v>
+      </c>
+      <c r="K15">
+        <v>0.1156186612576064</v>
+      </c>
+      <c r="L15">
+        <v>28.17</v>
+      </c>
+      <c r="M15">
+        <v>0.09101471727343147</v>
+      </c>
+      <c r="N15">
+        <v>100.84</v>
+      </c>
+      <c r="O15">
+        <v>0.1381489841986456</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="2">
+        <v>42800</v>
+      </c>
+      <c r="B16">
+        <v>846.61</v>
+      </c>
+      <c r="C16">
+        <v>0.007929043395440205</v>
+      </c>
+      <c r="D16">
+        <v>827.78</v>
+      </c>
+      <c r="E16">
+        <v>0.03662980727086018</v>
+      </c>
+      <c r="F16">
+        <v>64.27</v>
+      </c>
+      <c r="G16">
+        <v>0.01741332911192006</v>
+      </c>
+      <c r="H16">
+        <v>47.51</v>
+      </c>
+      <c r="I16">
+        <v>0.1103061462958634</v>
+      </c>
+      <c r="J16">
+        <v>88.86</v>
+      </c>
+      <c r="K16">
+        <v>0.009772727272727266</v>
+      </c>
+      <c r="L16">
+        <v>30.41</v>
+      </c>
+      <c r="M16">
+        <v>0.07951721689740854</v>
+      </c>
+      <c r="N16">
+        <v>102.31</v>
+      </c>
+      <c r="O16">
+        <v>0.01457754859182869</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="2">
+        <v>42829</v>
+      </c>
+      <c r="B17">
+        <v>906.83</v>
+      </c>
+      <c r="C17">
+        <v>0.07113074497112004</v>
+      </c>
+      <c r="D17">
+        <v>834.5700000000001</v>
+      </c>
+      <c r="E17">
+        <v>0.008202662543187911</v>
+      </c>
+      <c r="F17">
+        <v>65.73</v>
+      </c>
+      <c r="G17">
+        <v>0.0227166640734402</v>
+      </c>
+      <c r="H17">
+        <v>49.39</v>
+      </c>
+      <c r="I17">
+        <v>0.03957061671227113</v>
+      </c>
+      <c r="J17">
+        <v>92.23</v>
+      </c>
+      <c r="K17">
+        <v>0.03792482556830978</v>
+      </c>
+      <c r="L17">
+        <v>31.44</v>
+      </c>
+      <c r="M17">
+        <v>0.03387043735613293</v>
+      </c>
+      <c r="N17">
+        <v>107.52</v>
+      </c>
+      <c r="O17">
+        <v>0.05092366337601395</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="2">
+        <v>42859</v>
+      </c>
+      <c r="B18">
+        <v>937.53</v>
+      </c>
+      <c r="C18">
+        <v>0.03385419538391976</v>
+      </c>
+      <c r="D18">
+        <v>931.66</v>
+      </c>
+      <c r="E18">
+        <v>0.1163353583282407</v>
+      </c>
+      <c r="F18">
+        <v>68.81</v>
+      </c>
+      <c r="G18">
+        <v>0.04685835995740151</v>
+      </c>
+      <c r="H18">
+        <v>52.2</v>
+      </c>
+      <c r="I18">
+        <v>0.05689410811905238</v>
+      </c>
+      <c r="J18">
+        <v>92.81999999999999</v>
+      </c>
+      <c r="K18">
+        <v>0.006397050851132846</v>
+      </c>
+      <c r="L18">
+        <v>35.4</v>
+      </c>
+      <c r="M18">
+        <v>0.1259541984732824</v>
+      </c>
+      <c r="N18">
+        <v>115.86</v>
+      </c>
+      <c r="O18">
+        <v>0.07756696428571441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>